<commit_message>
Ajout init du rapport 3
Gestion des risques = Done
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine9.xlsx
+++ b/meeting/GestionHedbo_Semaine9.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Objet de la réunion : Hebdomadaire</t>
   </si>
@@ -76,13 +76,7 @@
     <t>Déplacement</t>
   </si>
   <si>
-    <t>Gestion des risques</t>
-  </si>
-  <si>
     <t>Dessin</t>
-  </si>
-  <si>
-    <t>22/3/2013</t>
   </si>
   <si>
     <t>04/04/2013</t>
@@ -323,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -365,6 +359,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -374,9 +378,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -389,16 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -782,21 +773,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="A2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -818,12 +809,12 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -842,257 +833,246 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="A9" s="20" t="s">
         <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>25</v>
-      </c>
+      <c r="A10" s="20"/>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="19"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+    <row r="12" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>7</v>
+      </c>
       <c r="B12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="7" t="s">
+      <c r="D16" s="12"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="17" t="s">
-        <v>10</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="D17" s="18"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>11</v>
+      <c r="A18" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="18"/>
+        <v>21</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>13</v>
-      </c>
+      <c r="A19" s="21"/>
       <c r="B19" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="D21" s="14"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+    <row r="22" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>16</v>
-      </c>
+      <c r="A23" s="20"/>
       <c r="B23" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="1"/>
+    <row r="26" spans="1:5" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A7:A9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout Hebdo semaine 9
</commit_message>
<xml_diff>
--- a/meeting/GestionHedbo_Semaine9.xlsx
+++ b/meeting/GestionHedbo_Semaine9.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Objet de la réunion : Hebdomadaire</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Test unitaire</t>
   </si>
   <si>
-    <t>Fixer caméra robot</t>
-  </si>
-  <si>
     <t>Diane</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Olivier</t>
   </si>
   <si>
-    <t>22/2/2013</t>
-  </si>
-  <si>
     <t>Développement logiciel</t>
   </si>
   <si>
@@ -88,18 +82,12 @@
     <t>Francis</t>
   </si>
   <si>
-    <t>22/04/2013</t>
-  </si>
-  <si>
     <t>Plans électriques</t>
   </si>
   <si>
     <t>Installation matérielle</t>
   </si>
   <si>
-    <t>22/03/2013</t>
-  </si>
-  <si>
     <t>Orientation robot</t>
   </si>
   <si>
@@ -112,16 +100,10 @@
     <t>Tableau: gestion de projet (interne): semaine du 18 mars 2013</t>
   </si>
   <si>
-    <t>Microcontrôleur (Antenne)</t>
-  </si>
-  <si>
-    <t>Microcontrôleur (Sonore)</t>
-  </si>
-  <si>
     <t>04/04/2014</t>
   </si>
   <si>
-    <t>Orientation robot(Support Diane)</t>
+    <t>Support</t>
   </si>
 </sst>
 </file>
@@ -132,7 +114,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -144,13 +126,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF008000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -185,12 +160,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,14 +171,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -317,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,29 +321,36 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -378,18 +360,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -773,21 +745,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -809,12 +781,12 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="A5" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -833,244 +805,199 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>23</v>
+      <c r="A9" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="D9" s="27"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="16"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="18"/>
+        <v>19</v>
+      </c>
+      <c r="D14" s="28"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>12</v>
+      </c>
       <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="17" t="s">
-        <v>10</v>
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="23"/>
       <c r="B17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>13</v>
+    <row r="18" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+    <row r="19" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+    <row r="20" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
       <c r="B20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+    <row r="21" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="1"/>
+    <row r="22" spans="1:5" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A7:A8"/>
   </mergeCells>

</xml_diff>